<commit_message>
UA added cucumber to the FW
</commit_message>
<xml_diff>
--- a/src/main/java/com/site/testdata/FreeCRM_Data.xlsx
+++ b/src/main/java/com/site/testdata/FreeCRM_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/654523255c32963a/Documents/Automation/Git/MavenPomTestFW/src/main/java/com/site/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_F25DC773A252ABDACC104895B99D71F25BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1C2F994-301E-4204-8E12-DF5EC63C6C21}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="11_F25DC773A252ABDACC104895B99D71F25BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE062CB2-2AE8-4FCC-A0D4-15DBFCB26E25}"/>
   <bookViews>
     <workbookView xWindow="29190" yWindow="-585" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,31 +36,31 @@
     <t>middlename</t>
   </si>
   <si>
-    <t>Jen</t>
-  </si>
-  <si>
-    <t>Socratis</t>
-  </si>
-  <si>
-    <t>Harry</t>
-  </si>
-  <si>
-    <t>Jane</t>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Marie</t>
+  </si>
+  <si>
+    <t>Davia</t>
+  </si>
+  <si>
+    <t>Jay</t>
+  </si>
+  <si>
+    <t>Alison</t>
+  </si>
+  <si>
+    <t>Connor</t>
   </si>
   <si>
     <t>Jones</t>
   </si>
   <si>
-    <t>alex</t>
-  </si>
-  <si>
-    <t>Smithson</t>
-  </si>
-  <si>
-    <t>Kane</t>
-  </si>
-  <si>
-    <t>Tihs</t>
+    <t>Palm</t>
+  </si>
+  <si>
+    <t>Jackson</t>
   </si>
 </sst>
 </file>
@@ -113,6 +113,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -408,29 +412,29 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UA experiementing with custom waits
</commit_message>
<xml_diff>
--- a/src/main/java/com/site/testdata/FreeCRM_Data.xlsx
+++ b/src/main/java/com/site/testdata/FreeCRM_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/654523255c32963a/Documents/Automation/Git/MavenPomTestFW/src/main/java/com/site/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="11_F25DC773A252ABDACC104895B99D71F25BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE062CB2-2AE8-4FCC-A0D4-15DBFCB26E25}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="11_F25DC773A252ABDACC104895B99D71F25BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CF13EA6-1484-41F5-9A3D-996B5788C8AC}"/>
   <bookViews>
     <workbookView xWindow="29190" yWindow="-585" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,15 +45,6 @@
     <t>Davia</t>
   </si>
   <si>
-    <t>Jay</t>
-  </si>
-  <si>
-    <t>Alison</t>
-  </si>
-  <si>
-    <t>Connor</t>
-  </si>
-  <si>
     <t>Jones</t>
   </si>
   <si>
@@ -61,6 +52,15 @@
   </si>
   <si>
     <t>Jackson</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>DEF</t>
+  </si>
+  <si>
+    <t>GHI</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,35 +406,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>